<commit_message>
Fixed a problem in 'help.xlsx' that prevented the help information to be correctly managed by 'populate_db'.
</commit_message>
<xml_diff>
--- a/b11_1/pgsql/help.xlsx
+++ b/b11_1/pgsql/help.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yann/Prog/Python/LBA-b11-1/b11_1/pgsql/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770CA520-F2F3-9641-B419-43F60B1FE88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF67060-189F-CF45-A44E-0243A4EC55E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="33120" windowHeight="25860" tabRatio="848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -406,9 +406,6 @@
     <t>Inline_help_EN</t>
   </si>
   <si>
-    <t>FR - Kurze Artikelbeschreibung f√ºr Bildschirmanzeige, Etiketten und Reports. F√ºr systemspezifische Items wird soweit als m√∂glich die Benennung des Originalherstellers √ºbernommen. F√ºr Normteile gelten die Vorgaben gem√§ss zivilen und milit√§rischen Normen. Der Materialkurztext wird grunds√§tzlich mit Sprachschl√ºssel DE und FR in der Beilage 11.1 erfasst. &lt;/br&gt;&lt;/br&gt;Bis zu 40 Stellen langer Text, der das Material n√§her bezeichnet. Der Materialkurztext ist die Bezeichnung des Materials. Es kann f√ºr beliebig viele Sprachen jeweils genau einen Kurztext geben. Siehe AFB NG ZID Kap. 4.3.1&lt;/br&gt;&lt;/br&gt;Falls der Lieferant den Kurztext in englisch anliefert, wird dieser hier eingepflegt. Das System schreibt diesen automatisch in den Kurztext EN.</t>
-  </si>
-  <si>
     <t>FR - Format</t>
   </si>
   <si>
@@ -418,18 +415,9 @@
     <t>EN - Format</t>
   </si>
   <si>
-    <t>DE - Eine Information √ºber das erwartete&lt;br/&gt;Format f√ºr den Feld 'BEGRU‚Äô.</t>
-  </si>
-  <si>
-    <t>EN - Eine Information √ºber das erwartete&lt;br/&gt;Format f√ºr den Feld 'BEGRU'.</t>
-  </si>
-  <si>
     <t>Obligatorisch bei SBM</t>
   </si>
   <si>
-    <t>Eine Info √ºber das Format&lt;br/&gt;f√ºr den Feld 'kennziffer_bamf'.</t>
-  </si>
-  <si>
     <t>Field</t>
   </si>
   <si>
@@ -691,9 +679,6 @@
     <t>&lt;/br&gt;Schlüssel, über den Sie das Material einer externen Warengruppe oder einer Warengruppe, die nach einer externen Systematik ermittelt wird, zuordnen können.</t>
   </si>
   <si>
-    <t>Wird ein Material mittels Lohnbearbeitungsbestellung zur Instandsetzung/Wartung geschickt, muss die Rechnungsanschrift der Firma nicht zwingend auch die Reparaturstelle sein. In diesen Fällen müssen entsprechende Reparaturlokationen angelegt und gepflegt werden.&lt;/br&gt;&lt;/br&gt;ACHTUNG - Dieses Feld ist ausschliesslich ein Informationsfeld!&lt;/br&gt;Die Reparaturlokation kann NICHT inital mittels B11.1 angelegt werden, sondern muss nach der Eröffnung des Materials vom Datenmanager LBA gesondert im PSD (Grunddaten 2 | Z-Felder) hinterlegt werden.</t>
-  </si>
-  <si>
     <t>werkzuordnung_1</t>
   </si>
   <si>
@@ -704,6 +689,21 @@
   </si>
   <si>
     <t>werkzuordnung_4</t>
+  </si>
+  <si>
+    <t>DE - Eine Information über das erwartete&lt;br/&gt;Format für den Feld 'BEGRU‚Äô.</t>
+  </si>
+  <si>
+    <t>EN - Eine Information über das erwartete&lt;br/&gt;Format für den Feld 'BEGRU'.</t>
+  </si>
+  <si>
+    <t>Eine Info über das Format&lt;br/&gt;für den Feld 'kennziffer_bamf'.</t>
+  </si>
+  <si>
+    <t>FR - Kurze Artikelbeschreibung für Bildschirmanzeige, Etiketten und Reports. für systemspezifische Items wird soweit als möglich die Benennung des Originalherstellers übernommen. für Normteile gelten die Vorgaben gemäss zivilen und militärischen Normen. Der Materialkurztext wird grundsätzlich mit Sprachschlüssel DE und FR in der Beilage 11.1 erfasst. &lt;/br&gt;&lt;/br&gt;Bis zu 40 Stellen langer Text, der das Material näher bezeichnet. Der Materialkurztext ist die Bezeichnung des Materials. Es kann für beliebig viele Sprachen jeweils genau einen Kurztext geben. Siehe AFB NG ZID Kap. 4.3.1&lt;/br&gt;&lt;/br&gt;Falls der Lieferant den Kurztext in englisch anliefert, wird dieser hier eingepflegt. Das System schreibt diesen automatisch in den Kurztext EN.</t>
+  </si>
+  <si>
+    <t>Wird ein Material mittels Lohnbearbeitungsbestellung zur Instandsetzung/Wartung geschickt, muss die Rechnungsanschrift der Firma nicht zwingend auch die Reparaturstelle sein. In diesen Fällen müssen entsprechende Reparaturlokationen angelegt und gepflegt werden.&lt;/br&gt;&lt;/br&gt;ACHTUNG - Dieses Feld ist ausschliesslich ein Informationsfeld!&lt;/br&gt;Die Reparaturlokation kann NICHT inital mittels B11.1 angelegt werden, sondern muss nach der Eröffnung des Materials vom Datenmanager LBA gesondert im PSD (Grunddaten 2 / Z-Felder) hinterlegt werden.</t>
   </si>
 </sst>
 </file>
@@ -1862,9 +1862,9 @@
   </sheetPr>
   <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="A29:XFD29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1876,7 +1876,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="40.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B1" t="s">
         <v>106</v>
@@ -1925,22 +1925,22 @@
         <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="120" customHeight="1" x14ac:dyDescent="0.2">
@@ -1948,7 +1948,7 @@
         <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>0</v>
@@ -1960,7 +1960,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>0</v>
@@ -1994,7 +1994,7 @@
         <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>0</v>
@@ -2006,7 +2006,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>0</v>
@@ -2017,7 +2017,7 @@
         <v>34</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>0</v>
@@ -2029,7 +2029,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>0</v>
@@ -2063,7 +2063,7 @@
         <v>35</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>0</v>
@@ -2075,7 +2075,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>0</v>
@@ -2086,7 +2086,7 @@
         <v>41</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>0</v>
@@ -2098,7 +2098,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>0</v>
@@ -2109,7 +2109,7 @@
         <v>55</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>0</v>
@@ -2121,7 +2121,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>0</v>
@@ -2132,7 +2132,7 @@
         <v>52</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>0</v>
@@ -2144,7 +2144,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>0</v>
@@ -2178,7 +2178,7 @@
         <v>54</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>0</v>
@@ -2190,7 +2190,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>0</v>
@@ -2247,7 +2247,7 @@
         <v>56</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>0</v>
@@ -2259,7 +2259,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>0</v>
@@ -2270,7 +2270,7 @@
         <v>58</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>0</v>
@@ -2282,7 +2282,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>0</v>
@@ -2293,7 +2293,7 @@
         <v>59</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>0</v>
@@ -2305,7 +2305,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>0</v>
@@ -2316,7 +2316,7 @@
         <v>85</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>0</v>
@@ -2328,7 +2328,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>0</v>
@@ -2339,7 +2339,7 @@
         <v>61</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>0</v>
@@ -2351,7 +2351,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>0</v>
@@ -2362,7 +2362,7 @@
         <v>62</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>0</v>
@@ -2374,7 +2374,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>0</v>
@@ -2385,7 +2385,7 @@
         <v>40</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>0</v>
@@ -2477,7 +2477,7 @@
         <v>42</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>0</v>
@@ -2489,7 +2489,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>0</v>
@@ -2500,7 +2500,7 @@
         <v>43</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>0</v>
@@ -2512,7 +2512,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>0</v>
@@ -2523,7 +2523,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>0</v>
@@ -2535,7 +2535,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>0</v>
@@ -2546,7 +2546,7 @@
         <v>57</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>0</v>
@@ -2558,7 +2558,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>0</v>
@@ -2569,7 +2569,7 @@
         <v>60</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>0</v>
@@ -2581,7 +2581,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>0</v>
@@ -2592,7 +2592,7 @@
         <v>49</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>0</v>
@@ -2604,7 +2604,7 @@
         <v>0</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>0</v>
@@ -2615,7 +2615,7 @@
         <v>45</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>0</v>
@@ -2627,7 +2627,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>0</v>
@@ -2638,7 +2638,7 @@
         <v>46</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>0</v>
@@ -2650,7 +2650,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>0</v>
@@ -2661,7 +2661,7 @@
         <v>47</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>0</v>
@@ -2673,7 +2673,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>0</v>
@@ -2684,7 +2684,7 @@
         <v>48</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>0</v>
@@ -2696,7 +2696,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>0</v>
@@ -2753,10 +2753,10 @@
         <v>69</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>116</v>
+        <v>207</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>0</v>
@@ -2765,10 +2765,10 @@
         <v>0</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>117</v>
+        <v>208</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="200" customHeight="1" x14ac:dyDescent="0.2">
@@ -2776,7 +2776,7 @@
         <v>90</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>0</v>
@@ -2788,7 +2788,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>0</v>
@@ -2811,7 +2811,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>0</v>
@@ -2822,7 +2822,7 @@
         <v>68</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>0</v>
@@ -2834,7 +2834,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>0</v>
@@ -2845,7 +2845,7 @@
         <v>65</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>0</v>
@@ -2857,7 +2857,7 @@
         <v>0</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>0</v>
@@ -2868,7 +2868,7 @@
         <v>92</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>0</v>
@@ -2880,7 +2880,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>0</v>
@@ -2891,7 +2891,7 @@
         <v>93</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>0</v>
@@ -2903,7 +2903,7 @@
         <v>0</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>0</v>
@@ -2914,7 +2914,7 @@
         <v>74</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>0</v>
@@ -2926,7 +2926,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>0</v>
@@ -2937,7 +2937,7 @@
         <v>94</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>0</v>
@@ -2949,7 +2949,7 @@
         <v>0</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>0</v>
@@ -2960,7 +2960,7 @@
         <v>75</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>0</v>
@@ -2972,7 +2972,7 @@
         <v>0</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>0</v>
@@ -2983,7 +2983,7 @@
         <v>73</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>0</v>
@@ -2995,7 +2995,7 @@
         <v>0</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>0</v>
@@ -3006,7 +3006,7 @@
         <v>67</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>0</v>
@@ -3018,7 +3018,7 @@
         <v>0</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>0</v>
@@ -3029,7 +3029,7 @@
         <v>76</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>0</v>
@@ -3041,7 +3041,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>0</v>
@@ -3052,7 +3052,7 @@
         <v>79</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>0</v>
@@ -3064,7 +3064,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>0</v>
@@ -3075,7 +3075,7 @@
         <v>77</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>0</v>
@@ -3087,7 +3087,7 @@
         <v>0</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>0</v>
@@ -3098,7 +3098,7 @@
         <v>81</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>0</v>
@@ -3110,7 +3110,7 @@
         <v>0</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>0</v>
@@ -3118,10 +3118,10 @@
     </row>
     <row r="55" spans="1:7" ht="140" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>0</v>
@@ -3133,7 +3133,7 @@
         <v>0</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>0</v>
@@ -3141,10 +3141,10 @@
     </row>
     <row r="56" spans="1:7" ht="140" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>0</v>
@@ -3156,7 +3156,7 @@
         <v>0</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>0</v>
@@ -3164,10 +3164,10 @@
     </row>
     <row r="57" spans="1:7" ht="140" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>0</v>
@@ -3179,7 +3179,7 @@
         <v>0</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>0</v>
@@ -3187,10 +3187,10 @@
     </row>
     <row r="58" spans="1:7" ht="140" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>0</v>
@@ -3202,7 +3202,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>0</v>
@@ -3213,7 +3213,7 @@
         <v>91</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>0</v>
@@ -3225,7 +3225,7 @@
         <v>0</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>0</v>
@@ -3236,7 +3236,7 @@
         <v>80</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>0</v>
@@ -3248,7 +3248,7 @@
         <v>0</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>0</v>
@@ -3259,7 +3259,7 @@
         <v>89</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>0</v>
@@ -3271,7 +3271,7 @@
         <v>0</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>0</v>
@@ -3282,7 +3282,7 @@
         <v>82</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>0</v>
@@ -3294,7 +3294,7 @@
         <v>0</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>0</v>
@@ -3305,7 +3305,7 @@
         <v>83</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>0</v>
@@ -3317,7 +3317,7 @@
         <v>0</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>0</v>
@@ -3340,7 +3340,7 @@
         <v>0</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>0</v>
@@ -3351,7 +3351,7 @@
         <v>78</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>0</v>
@@ -3363,7 +3363,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>0</v>
@@ -3374,7 +3374,7 @@
         <v>96</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>0</v>
@@ -3386,7 +3386,7 @@
         <v>0</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>0</v>
@@ -3397,7 +3397,7 @@
         <v>84</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>0</v>
@@ -3409,7 +3409,7 @@
         <v>0</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>0</v>
@@ -3420,7 +3420,7 @@
         <v>70</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>0</v>
@@ -3432,7 +3432,7 @@
         <v>0</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>0</v>
@@ -3443,7 +3443,7 @@
         <v>71</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>0</v>
@@ -3455,7 +3455,7 @@
         <v>0</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>0</v>
@@ -3466,7 +3466,7 @@
         <v>72</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>0</v>
@@ -3478,7 +3478,7 @@
         <v>0</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>0</v>
@@ -3489,10 +3489,10 @@
         <v>2</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>0</v>
@@ -3501,7 +3501,7 @@
         <v>0</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>0</v>
@@ -3512,7 +3512,7 @@
         <v>3</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>0</v>
@@ -3524,7 +3524,7 @@
         <v>0</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>0</v>
@@ -3547,7 +3547,7 @@
         <v>0</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>0</v>
@@ -3570,7 +3570,7 @@
         <v>0</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>0</v>
@@ -3593,7 +3593,7 @@
         <v>0</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>0</v>
@@ -3616,7 +3616,7 @@
         <v>0</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>0</v>
@@ -3639,7 +3639,7 @@
         <v>0</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>0</v>
@@ -3650,7 +3650,7 @@
         <v>88</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>0</v>
@@ -3662,7 +3662,7 @@
         <v>0</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>0</v>
@@ -3673,7 +3673,7 @@
         <v>102</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>0</v>
@@ -3685,7 +3685,7 @@
         <v>0</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>0</v>
@@ -3696,7 +3696,7 @@
         <v>103</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>0</v>
@@ -3708,7 +3708,7 @@
         <v>0</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>0</v>
@@ -3722,7 +3722,7 @@
         <v>13</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>119</v>
+        <v>209</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>0</v>
@@ -3731,7 +3731,7 @@
         <v>0</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>0</v>
@@ -3754,7 +3754,7 @@
         <v>0</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>0</v>
@@ -3765,7 +3765,7 @@
         <v>104</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>0</v>
@@ -3777,7 +3777,7 @@
         <v>0</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>0</v>
@@ -3788,7 +3788,7 @@
         <v>105</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>0</v>
@@ -3800,7 +3800,7 @@
         <v>0</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>0</v>

</xml_diff>